<commit_message>
calculator prices changed to actual
</commit_message>
<xml_diff>
--- a/files/auto_moskva_yakutsk.xlsx
+++ b/files/auto_moskva_yakutsk.xlsx
@@ -691,7 +691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -702,7 +702,7 @@
   <dimension ref="A3:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -742,13 +742,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="9">
-        <v>9600</v>
+        <v>8500</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="12">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24.95" customHeight="1">
@@ -756,13 +756,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="10">
-        <v>9200</v>
+        <v>8200</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="13">
-        <v>42.5</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="24.95" customHeight="1">
@@ -770,13 +770,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="10">
-        <v>8900</v>
+        <v>8000</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="13">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="24.95" customHeight="1">
@@ -784,13 +784,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="10">
-        <v>8700</v>
+        <v>7800</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="13">
-        <v>40</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1">
@@ -798,13 +798,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="10">
-        <v>8600</v>
+        <v>7600</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="13">
-        <v>39.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="24.95" customHeight="1" thickBot="1">
@@ -812,13 +812,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="11">
-        <v>8500</v>
+        <v>7500</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="14">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="24.95" customHeight="1">

</xml_diff>